<commit_message>
training and test sets for credit sales
training contains 80% of all observations and test 20%
</commit_message>
<xml_diff>
--- a/datasets/Credit_Sales_Trening.xlsx
+++ b/datasets/Credit_Sales_Trening.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asia0\Desktop\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB8D1974-5B01-4297-BA05-32141B16AF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1A77884-122B-4A35-A522-32251F342A9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{9A620B74-42BC-47CE-8852-8F339195974B}"/>
   </bookViews>
@@ -431,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D56A674B-B062-4E83-8352-0DFEBC2570FE}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:H81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J43" sqref="J43"/>
+      <selection activeCell="J78" sqref="J78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1120,392 +1120,392 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
-        <v>572010</v>
+        <v>110060</v>
       </c>
       <c r="B27" s="1">
-        <v>1391497</v>
+        <v>856010</v>
       </c>
       <c r="C27" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D27" s="1">
-        <v>46000</v>
+        <v>10000</v>
       </c>
       <c r="E27" s="1">
         <v>1</v>
       </c>
       <c r="F27" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G27" s="1">
         <v>0</v>
       </c>
       <c r="H27" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
-        <v>390500</v>
+        <v>150010</v>
       </c>
       <c r="B28" s="1">
-        <v>600072</v>
+        <v>840074</v>
       </c>
       <c r="C28" s="1">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D28" s="1">
-        <v>35000</v>
+        <v>50000</v>
       </c>
       <c r="E28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F28" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="1">
         <v>0</v>
       </c>
       <c r="H28" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
-        <v>300211</v>
+        <v>165043</v>
       </c>
       <c r="B29" s="1">
-        <v>2740395</v>
+        <v>990900</v>
       </c>
       <c r="C29" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D29" s="1">
-        <v>0</v>
+        <v>15000</v>
       </c>
       <c r="E29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F29" s="1">
         <v>1</v>
       </c>
       <c r="G29" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H29" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
-        <v>970740</v>
+        <v>200500</v>
       </c>
       <c r="B30" s="1">
-        <v>1703040</v>
+        <v>1001003</v>
       </c>
       <c r="C30" s="1">
         <v>6</v>
       </c>
       <c r="D30" s="1">
-        <v>240000</v>
+        <v>0</v>
       </c>
       <c r="E30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H30" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
-        <v>500702</v>
+        <v>100309</v>
       </c>
       <c r="B31" s="1">
-        <v>1103051</v>
+        <v>598000</v>
       </c>
       <c r="C31" s="1">
+        <v>7</v>
+      </c>
+      <c r="D31" s="1">
+        <v>56000</v>
+      </c>
+      <c r="E31" s="1">
+        <v>0</v>
+      </c>
+      <c r="F31" s="1">
+        <v>1</v>
+      </c>
+      <c r="G31" s="1">
+        <v>1</v>
+      </c>
+      <c r="H31" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="2">
+        <v>99000</v>
+      </c>
+      <c r="B32" s="2">
+        <v>841015</v>
+      </c>
+      <c r="C32" s="2">
+        <v>6</v>
+      </c>
+      <c r="D32" s="2">
+        <v>10400</v>
+      </c>
+      <c r="E32" s="2">
+        <v>1</v>
+      </c>
+      <c r="F32" s="2">
+        <v>1</v>
+      </c>
+      <c r="G32" s="2">
+        <v>0</v>
+      </c>
+      <c r="H32" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A33" s="2">
+        <v>50100</v>
+      </c>
+      <c r="B33" s="2">
+        <v>750700</v>
+      </c>
+      <c r="C33" s="2">
         <v>8</v>
       </c>
-      <c r="D31" s="1">
-        <v>6030</v>
-      </c>
-      <c r="E31" s="1">
-        <v>0</v>
-      </c>
-      <c r="F31" s="1">
-        <v>1</v>
-      </c>
-      <c r="G31" s="1">
-        <v>0</v>
-      </c>
-      <c r="H31" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="1">
-        <v>356000</v>
-      </c>
-      <c r="B32" s="1">
-        <v>830012</v>
-      </c>
-      <c r="C32" s="1">
-        <v>6</v>
-      </c>
-      <c r="D32" s="1">
-        <v>0</v>
-      </c>
-      <c r="E32" s="1">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1">
-        <v>1</v>
-      </c>
-      <c r="G32" s="1">
-        <v>0</v>
-      </c>
-      <c r="H32" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="1">
-        <v>204070</v>
-      </c>
-      <c r="B33" s="1">
-        <v>712000</v>
-      </c>
-      <c r="C33" s="1">
+      <c r="D33" s="2">
+        <v>20000</v>
+      </c>
+      <c r="E33" s="2">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2">
+        <v>0</v>
+      </c>
+      <c r="H33" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="2">
+        <v>140700</v>
+      </c>
+      <c r="B34" s="2">
+        <v>953000</v>
+      </c>
+      <c r="C34" s="2">
+        <v>7</v>
+      </c>
+      <c r="D34" s="2">
+        <v>25000</v>
+      </c>
+      <c r="E34" s="2">
+        <v>1</v>
+      </c>
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2">
+        <v>1</v>
+      </c>
+      <c r="H34" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="2">
+        <v>190280</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1008033</v>
+      </c>
+      <c r="C35" s="2">
+        <v>6</v>
+      </c>
+      <c r="D35" s="2">
+        <v>0</v>
+      </c>
+      <c r="E35" s="2">
+        <v>1</v>
+      </c>
+      <c r="F35" s="2">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2">
+        <v>0</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="2">
+        <v>100350</v>
+      </c>
+      <c r="B36" s="2">
+        <v>602062</v>
+      </c>
+      <c r="C36" s="2">
+        <v>7</v>
+      </c>
+      <c r="D36" s="2">
+        <v>6000</v>
+      </c>
+      <c r="E36" s="2">
+        <v>0</v>
+      </c>
+      <c r="F36" s="2">
+        <v>1</v>
+      </c>
+      <c r="G36" s="2">
+        <v>1</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="2">
+        <v>203990</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1500638</v>
+      </c>
+      <c r="C37" s="2">
+        <v>12</v>
+      </c>
+      <c r="D37" s="2">
+        <v>200000</v>
+      </c>
+      <c r="E37" s="2">
+        <v>1</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0</v>
+      </c>
+      <c r="G37" s="2">
+        <v>1</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="2">
+        <v>90462</v>
+      </c>
+      <c r="B38" s="2">
+        <v>610742</v>
+      </c>
+      <c r="C38" s="2">
+        <v>6</v>
+      </c>
+      <c r="D38" s="2">
+        <v>75000</v>
+      </c>
+      <c r="E38" s="2">
+        <v>0</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0</v>
+      </c>
+      <c r="G38" s="2">
+        <v>0</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A39" s="2">
+        <v>160390</v>
+      </c>
+      <c r="B39" s="2">
+        <v>2134003</v>
+      </c>
+      <c r="C39" s="2">
+        <v>10</v>
+      </c>
+      <c r="D39" s="2">
+        <v>80100</v>
+      </c>
+      <c r="E39" s="2">
+        <v>1</v>
+      </c>
+      <c r="F39" s="2">
+        <v>1</v>
+      </c>
+      <c r="G39" s="2">
+        <v>0</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="2">
+        <v>340010</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1870481</v>
+      </c>
+      <c r="C40" s="2">
+        <v>7</v>
+      </c>
+      <c r="D40" s="2">
+        <v>670000</v>
+      </c>
+      <c r="E40" s="2">
+        <v>0</v>
+      </c>
+      <c r="F40" s="2">
+        <v>1</v>
+      </c>
+      <c r="G40" s="2">
+        <v>1</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A41" s="2">
+        <v>190500</v>
+      </c>
+      <c r="B41" s="2">
+        <v>3200100</v>
+      </c>
+      <c r="C41" s="2">
         <v>8</v>
       </c>
-      <c r="D33" s="1">
-        <v>3000</v>
-      </c>
-      <c r="E33" s="1">
-        <v>1</v>
-      </c>
-      <c r="F33" s="1">
-        <v>1</v>
-      </c>
-      <c r="G33" s="1">
-        <v>0</v>
-      </c>
-      <c r="H33" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="1">
-        <v>230000</v>
-      </c>
-      <c r="B34" s="1">
-        <v>954180</v>
-      </c>
-      <c r="C34" s="1">
-        <v>6</v>
-      </c>
-      <c r="D34" s="1">
-        <v>1600</v>
-      </c>
-      <c r="E34" s="1">
-        <v>0</v>
-      </c>
-      <c r="F34" s="1">
-        <v>1</v>
-      </c>
-      <c r="G34" s="1">
-        <v>0</v>
-      </c>
-      <c r="H34" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="1">
-        <v>208060</v>
-      </c>
-      <c r="B35" s="1">
-        <v>1000100</v>
-      </c>
-      <c r="C35" s="1">
-        <v>9</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0</v>
-      </c>
-      <c r="E35" s="1">
-        <v>1</v>
-      </c>
-      <c r="F35" s="1">
-        <v>0</v>
-      </c>
-      <c r="G35" s="1">
-        <v>0</v>
-      </c>
-      <c r="H35" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="1">
-        <v>182020</v>
-      </c>
-      <c r="B36" s="1">
-        <v>500492</v>
-      </c>
-      <c r="C36" s="1">
-        <v>7</v>
-      </c>
-      <c r="D36" s="1">
-        <v>0</v>
-      </c>
-      <c r="E36" s="1">
-        <v>0</v>
-      </c>
-      <c r="F36" s="1">
-        <v>1</v>
-      </c>
-      <c r="G36" s="1">
-        <v>0</v>
-      </c>
-      <c r="H36" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="1">
-        <v>250045</v>
-      </c>
-      <c r="B37" s="1">
-        <v>843060</v>
-      </c>
-      <c r="C37" s="1">
-        <v>6</v>
-      </c>
-      <c r="D37" s="1">
-        <v>0</v>
-      </c>
-      <c r="E37" s="1">
-        <v>1</v>
-      </c>
-      <c r="F37" s="1">
-        <v>1</v>
-      </c>
-      <c r="G37" s="1">
-        <v>0</v>
-      </c>
-      <c r="H37" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="1">
-        <v>198043</v>
-      </c>
-      <c r="B38" s="1">
-        <v>720023</v>
-      </c>
-      <c r="C38" s="1">
-        <v>7</v>
-      </c>
-      <c r="D38" s="1">
-        <v>2000</v>
-      </c>
-      <c r="E38" s="1">
-        <v>1</v>
-      </c>
-      <c r="F38" s="1">
-        <v>1</v>
-      </c>
-      <c r="G38" s="1">
-        <v>0</v>
-      </c>
-      <c r="H38" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="1">
-        <v>205502</v>
-      </c>
-      <c r="B39" s="1">
-        <v>903000</v>
-      </c>
-      <c r="C39" s="1">
-        <v>6</v>
-      </c>
-      <c r="D39" s="1">
-        <v>1000</v>
-      </c>
-      <c r="E39" s="1">
-        <v>0</v>
-      </c>
-      <c r="F39" s="1">
-        <v>1</v>
-      </c>
-      <c r="G39" s="1">
-        <v>0</v>
-      </c>
-      <c r="H39" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="1">
-        <v>200620</v>
-      </c>
-      <c r="B40" s="1">
-        <v>1047500</v>
-      </c>
-      <c r="C40" s="1">
-        <v>9</v>
-      </c>
-      <c r="D40" s="1">
-        <v>0</v>
-      </c>
-      <c r="E40" s="1">
-        <v>1</v>
-      </c>
-      <c r="F40" s="1">
-        <v>0</v>
-      </c>
-      <c r="G40" s="1">
-        <v>0</v>
-      </c>
-      <c r="H40" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" s="1">
-        <v>110020</v>
-      </c>
-      <c r="B41" s="1">
-        <v>470490</v>
-      </c>
-      <c r="C41" s="1">
-        <v>7</v>
-      </c>
-      <c r="D41" s="1">
-        <v>0</v>
-      </c>
-      <c r="E41" s="1">
-        <v>0</v>
-      </c>
-      <c r="F41" s="1">
-        <v>1</v>
-      </c>
-      <c r="G41" s="1">
-        <v>0</v>
-      </c>
-      <c r="H41" s="1">
-        <v>1</v>
+      <c r="D41" s="2">
+        <v>51100</v>
+      </c>
+      <c r="E41" s="2">
+        <v>1</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0</v>
+      </c>
+      <c r="G41" s="2">
+        <v>1</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
@@ -1765,6 +1765,786 @@
         <v>0</v>
       </c>
       <c r="H51" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="1">
+        <v>572010</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1391497</v>
+      </c>
+      <c r="C52" s="1">
+        <v>11</v>
+      </c>
+      <c r="D52" s="1">
+        <v>46000</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1">
+        <v>0</v>
+      </c>
+      <c r="G52" s="1">
+        <v>0</v>
+      </c>
+      <c r="H52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="1">
+        <v>390500</v>
+      </c>
+      <c r="B53" s="1">
+        <v>600072</v>
+      </c>
+      <c r="C53" s="1">
+        <v>6</v>
+      </c>
+      <c r="D53" s="1">
+        <v>35000</v>
+      </c>
+      <c r="E53" s="1">
+        <v>0</v>
+      </c>
+      <c r="F53" s="1">
+        <v>0</v>
+      </c>
+      <c r="G53" s="1">
+        <v>0</v>
+      </c>
+      <c r="H53" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A54" s="1">
+        <v>300211</v>
+      </c>
+      <c r="B54" s="1">
+        <v>2740395</v>
+      </c>
+      <c r="C54" s="1">
+        <v>10</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <v>0</v>
+      </c>
+      <c r="F54" s="1">
+        <v>1</v>
+      </c>
+      <c r="G54" s="1">
+        <v>0</v>
+      </c>
+      <c r="H54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A55" s="1">
+        <v>970740</v>
+      </c>
+      <c r="B55" s="1">
+        <v>1703040</v>
+      </c>
+      <c r="C55" s="1">
+        <v>6</v>
+      </c>
+      <c r="D55" s="1">
+        <v>240000</v>
+      </c>
+      <c r="E55" s="1">
+        <v>0</v>
+      </c>
+      <c r="F55" s="1">
+        <v>0</v>
+      </c>
+      <c r="G55" s="1">
+        <v>0</v>
+      </c>
+      <c r="H55" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A56" s="1">
+        <v>500702</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1103051</v>
+      </c>
+      <c r="C56" s="1">
+        <v>8</v>
+      </c>
+      <c r="D56" s="1">
+        <v>6030</v>
+      </c>
+      <c r="E56" s="1">
+        <v>0</v>
+      </c>
+      <c r="F56" s="1">
+        <v>1</v>
+      </c>
+      <c r="G56" s="1">
+        <v>0</v>
+      </c>
+      <c r="H56" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" s="1">
+        <v>356000</v>
+      </c>
+      <c r="B57" s="1">
+        <v>830012</v>
+      </c>
+      <c r="C57" s="1">
+        <v>6</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0</v>
+      </c>
+      <c r="E57" s="1">
+        <v>1</v>
+      </c>
+      <c r="F57" s="1">
+        <v>1</v>
+      </c>
+      <c r="G57" s="1">
+        <v>0</v>
+      </c>
+      <c r="H57" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A58" s="1">
+        <v>204070</v>
+      </c>
+      <c r="B58" s="1">
+        <v>712000</v>
+      </c>
+      <c r="C58" s="1">
+        <v>8</v>
+      </c>
+      <c r="D58" s="1">
+        <v>3000</v>
+      </c>
+      <c r="E58" s="1">
+        <v>1</v>
+      </c>
+      <c r="F58" s="1">
+        <v>1</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A59" s="1">
+        <v>230000</v>
+      </c>
+      <c r="B59" s="1">
+        <v>954180</v>
+      </c>
+      <c r="C59" s="1">
+        <v>6</v>
+      </c>
+      <c r="D59" s="1">
+        <v>1600</v>
+      </c>
+      <c r="E59" s="1">
+        <v>0</v>
+      </c>
+      <c r="F59" s="1">
+        <v>1</v>
+      </c>
+      <c r="G59" s="1">
+        <v>0</v>
+      </c>
+      <c r="H59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A60" s="1">
+        <v>208060</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1000100</v>
+      </c>
+      <c r="C60" s="1">
+        <v>9</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+      <c r="F60" s="1">
+        <v>0</v>
+      </c>
+      <c r="G60" s="1">
+        <v>0</v>
+      </c>
+      <c r="H60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A61" s="1">
+        <v>182020</v>
+      </c>
+      <c r="B61" s="1">
+        <v>500492</v>
+      </c>
+      <c r="C61" s="1">
+        <v>7</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1">
+        <v>0</v>
+      </c>
+      <c r="F61" s="1">
+        <v>1</v>
+      </c>
+      <c r="G61" s="1">
+        <v>0</v>
+      </c>
+      <c r="H61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A62" s="1">
+        <v>250045</v>
+      </c>
+      <c r="B62" s="1">
+        <v>843060</v>
+      </c>
+      <c r="C62" s="1">
+        <v>6</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1">
+        <v>1</v>
+      </c>
+      <c r="F62" s="1">
+        <v>1</v>
+      </c>
+      <c r="G62" s="1">
+        <v>0</v>
+      </c>
+      <c r="H62" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A63" s="1">
+        <v>198043</v>
+      </c>
+      <c r="B63" s="1">
+        <v>720023</v>
+      </c>
+      <c r="C63" s="1">
+        <v>7</v>
+      </c>
+      <c r="D63" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E63" s="1">
+        <v>1</v>
+      </c>
+      <c r="F63" s="1">
+        <v>1</v>
+      </c>
+      <c r="G63" s="1">
+        <v>0</v>
+      </c>
+      <c r="H63" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A64" s="1">
+        <v>205502</v>
+      </c>
+      <c r="B64" s="1">
+        <v>903000</v>
+      </c>
+      <c r="C64" s="1">
+        <v>6</v>
+      </c>
+      <c r="D64" s="1">
+        <v>1000</v>
+      </c>
+      <c r="E64" s="1">
+        <v>0</v>
+      </c>
+      <c r="F64" s="1">
+        <v>1</v>
+      </c>
+      <c r="G64" s="1">
+        <v>0</v>
+      </c>
+      <c r="H64" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" s="1">
+        <v>200620</v>
+      </c>
+      <c r="B65" s="1">
+        <v>1047500</v>
+      </c>
+      <c r="C65" s="1">
+        <v>9</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>1</v>
+      </c>
+      <c r="F65" s="1">
+        <v>0</v>
+      </c>
+      <c r="G65" s="1">
+        <v>0</v>
+      </c>
+      <c r="H65" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" s="1">
+        <v>110020</v>
+      </c>
+      <c r="B66" s="1">
+        <v>470490</v>
+      </c>
+      <c r="C66" s="1">
+        <v>7</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1">
+        <v>0</v>
+      </c>
+      <c r="F66" s="1">
+        <v>1</v>
+      </c>
+      <c r="G66" s="1">
+        <v>0</v>
+      </c>
+      <c r="H66" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67" s="1">
+        <v>356004</v>
+      </c>
+      <c r="B67" s="1">
+        <v>830003</v>
+      </c>
+      <c r="C67" s="1">
+        <v>6</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1">
+        <v>1</v>
+      </c>
+      <c r="F67" s="1">
+        <v>1</v>
+      </c>
+      <c r="G67" s="1">
+        <v>0</v>
+      </c>
+      <c r="H67" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68" s="1">
+        <v>204010</v>
+      </c>
+      <c r="B68" s="1">
+        <v>712081</v>
+      </c>
+      <c r="C68" s="1">
+        <v>6</v>
+      </c>
+      <c r="D68" s="1">
+        <v>3000</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1</v>
+      </c>
+      <c r="F68" s="1">
+        <v>1</v>
+      </c>
+      <c r="G68" s="1">
+        <v>0</v>
+      </c>
+      <c r="H68" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69" s="1">
+        <v>230073</v>
+      </c>
+      <c r="B69" s="1">
+        <v>954000</v>
+      </c>
+      <c r="C69" s="1">
+        <v>6</v>
+      </c>
+      <c r="D69" s="1">
+        <v>1600</v>
+      </c>
+      <c r="E69" s="1">
+        <v>0</v>
+      </c>
+      <c r="F69" s="1">
+        <v>1</v>
+      </c>
+      <c r="G69" s="1">
+        <v>0</v>
+      </c>
+      <c r="H69" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70" s="1">
+        <v>208091</v>
+      </c>
+      <c r="B70" s="1">
+        <v>1000100</v>
+      </c>
+      <c r="C70" s="1">
+        <v>9</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0</v>
+      </c>
+      <c r="E70" s="1">
+        <v>1</v>
+      </c>
+      <c r="F70" s="1">
+        <v>0</v>
+      </c>
+      <c r="G70" s="1">
+        <v>0</v>
+      </c>
+      <c r="H70" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A71" s="1">
+        <v>182000</v>
+      </c>
+      <c r="B71" s="1">
+        <v>500026</v>
+      </c>
+      <c r="C71" s="1">
+        <v>7</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0</v>
+      </c>
+      <c r="E71" s="1">
+        <v>0</v>
+      </c>
+      <c r="F71" s="1">
+        <v>1</v>
+      </c>
+      <c r="G71" s="1">
+        <v>0</v>
+      </c>
+      <c r="H71" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A72" s="1">
+        <v>572030</v>
+      </c>
+      <c r="B72" s="1">
+        <v>1390390</v>
+      </c>
+      <c r="C72" s="1">
+        <v>11</v>
+      </c>
+      <c r="D72" s="1">
+        <v>46000</v>
+      </c>
+      <c r="E72" s="1">
+        <v>1</v>
+      </c>
+      <c r="F72" s="1">
+        <v>0</v>
+      </c>
+      <c r="G72" s="1">
+        <v>0</v>
+      </c>
+      <c r="H72" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" s="1">
+        <v>390500</v>
+      </c>
+      <c r="B73" s="1">
+        <v>600072</v>
+      </c>
+      <c r="C73" s="1">
+        <v>6</v>
+      </c>
+      <c r="D73" s="1">
+        <v>35000</v>
+      </c>
+      <c r="E73" s="1">
+        <v>0</v>
+      </c>
+      <c r="F73" s="1">
+        <v>0</v>
+      </c>
+      <c r="G73" s="1">
+        <v>0</v>
+      </c>
+      <c r="H73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" s="1">
+        <v>300730</v>
+      </c>
+      <c r="B74" s="1">
+        <v>2740060</v>
+      </c>
+      <c r="C74" s="1">
+        <v>10</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0</v>
+      </c>
+      <c r="E74" s="1">
+        <v>0</v>
+      </c>
+      <c r="F74" s="1">
+        <v>1</v>
+      </c>
+      <c r="G74" s="1">
+        <v>0</v>
+      </c>
+      <c r="H74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75" s="1">
+        <v>970038</v>
+      </c>
+      <c r="B75" s="1">
+        <v>1703005</v>
+      </c>
+      <c r="C75" s="1">
+        <v>6</v>
+      </c>
+      <c r="D75" s="1">
+        <v>240000</v>
+      </c>
+      <c r="E75" s="1">
+        <v>0</v>
+      </c>
+      <c r="F75" s="1">
+        <v>0</v>
+      </c>
+      <c r="G75" s="1">
+        <v>0</v>
+      </c>
+      <c r="H75" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" s="1">
+        <v>500700</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1103017</v>
+      </c>
+      <c r="C76" s="1">
+        <v>8</v>
+      </c>
+      <c r="D76" s="1">
+        <v>6030</v>
+      </c>
+      <c r="E76" s="1">
+        <v>0</v>
+      </c>
+      <c r="F76" s="1">
+        <v>1</v>
+      </c>
+      <c r="G76" s="1">
+        <v>0</v>
+      </c>
+      <c r="H76" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" s="1">
+        <v>502000</v>
+      </c>
+      <c r="B77" s="1">
+        <v>1500000</v>
+      </c>
+      <c r="C77" s="1">
+        <v>6</v>
+      </c>
+      <c r="D77" s="1">
+        <v>50500</v>
+      </c>
+      <c r="E77" s="1">
+        <v>1</v>
+      </c>
+      <c r="F77" s="1">
+        <v>0</v>
+      </c>
+      <c r="G77" s="1">
+        <v>0</v>
+      </c>
+      <c r="H77" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" s="1">
+        <v>300500</v>
+      </c>
+      <c r="B78" s="1">
+        <v>580000</v>
+      </c>
+      <c r="C78" s="1">
+        <v>6</v>
+      </c>
+      <c r="D78" s="1">
+        <v>100100</v>
+      </c>
+      <c r="E78" s="1">
+        <v>0</v>
+      </c>
+      <c r="F78" s="1">
+        <v>0</v>
+      </c>
+      <c r="G78" s="1">
+        <v>0</v>
+      </c>
+      <c r="H78" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" s="1">
+        <v>184500</v>
+      </c>
+      <c r="B79" s="1">
+        <v>2607000</v>
+      </c>
+      <c r="C79" s="1">
+        <v>10</v>
+      </c>
+      <c r="D79" s="1">
+        <v>0</v>
+      </c>
+      <c r="E79" s="1">
+        <v>0</v>
+      </c>
+      <c r="F79" s="1">
+        <v>1</v>
+      </c>
+      <c r="G79" s="1">
+        <v>0</v>
+      </c>
+      <c r="H79" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" s="1">
+        <v>950670</v>
+      </c>
+      <c r="B80" s="1">
+        <v>1750862</v>
+      </c>
+      <c r="C80" s="1">
+        <v>6</v>
+      </c>
+      <c r="D80" s="1">
+        <v>270000</v>
+      </c>
+      <c r="E80" s="1">
+        <v>0</v>
+      </c>
+      <c r="F80" s="1">
+        <v>0</v>
+      </c>
+      <c r="G80" s="1">
+        <v>0</v>
+      </c>
+      <c r="H80" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A81" s="1">
+        <v>409500</v>
+      </c>
+      <c r="B81" s="1">
+        <v>1130380</v>
+      </c>
+      <c r="C81" s="1">
+        <v>8</v>
+      </c>
+      <c r="D81" s="1">
+        <v>6000</v>
+      </c>
+      <c r="E81" s="1">
+        <v>0</v>
+      </c>
+      <c r="F81" s="1">
+        <v>1</v>
+      </c>
+      <c r="G81" s="1">
+        <v>0</v>
+      </c>
+      <c r="H81" s="1">
         <v>1</v>
       </c>
     </row>

</xml_diff>